<commit_message>
Test updated.  Everything works as advertised.
</commit_message>
<xml_diff>
--- a/Project 1/boundary_plot.xlsx
+++ b/Project 1/boundary_plot.xlsx
@@ -250,36 +250,72 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.0797547059999999</c:v>
+                  <c:v>0.57911711399999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0989297840000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.117740331</c:v>
+                  <c:v>1.2893761690000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.571012791</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5981794899999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.716910758</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7991717709999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8093830630000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8783875750000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>Sheet1!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.62559920199999997</c:v>
+                  <c:v>1.508560248</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.196824202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1391688320000002</c:v>
+                  <c:v>0.90952006200000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2674740000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.71560431400000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.110969495</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.473503489</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.09224725</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.99794760900000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,42 +735,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.99751234200000005</c:v>
+                  <c:v>0.83525727400000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0581777880000001</c:v>
+                  <c:v>1.019497222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.081908849</c:v>
+                  <c:v>1.2053758809999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1116785890000001</c:v>
+                  <c:v>1.5209354500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5856842099999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5990193020000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.666065028</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7490675929999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.844634624</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2295364069999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.448862278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7.678653712</c:v>
+                  <c:v>2.613833101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.857649205</c:v>
+                  <c:v>2.126262401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5988149329999999</c:v>
+                  <c:v>0.39888146499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4539716789999999</c:v>
+                  <c:v>0.94678173200000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86914396000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.25382832700000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0501666460000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48787993299999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.36900263599999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4105133000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.329382168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2154,16 +2232,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2190,16 +2268,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>318135</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>127635</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>70485</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>127635</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>74295</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2528,10 +2606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,24 +2636,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.99751234200000005</v>
+        <v>0.83525727400000005</v>
       </c>
       <c r="B2">
-        <v>7.678653712</v>
+        <v>2.613833101</v>
       </c>
       <c r="D2">
-        <v>1.0797547059999999</v>
+        <v>0.57911711399999999</v>
       </c>
       <c r="E2">
-        <v>-0.62559920199999997</v>
+        <v>1.508560248</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.0581777880000001</v>
+        <v>1.019497222</v>
       </c>
       <c r="B3">
-        <v>2.857649205</v>
+        <v>2.126262401</v>
       </c>
       <c r="D3">
         <v>1.0989297840000001</v>
@@ -2586,29 +2664,121 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.081908849</v>
+        <v>1.2053758809999999</v>
       </c>
       <c r="B4">
-        <v>2.5988149329999999</v>
+        <v>0.39888146499999999</v>
       </c>
       <c r="D4">
-        <v>1.117740331</v>
+        <v>1.2893761690000001</v>
       </c>
       <c r="E4">
-        <v>-2.1391688320000002</v>
+        <v>0.90952006200000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1.1116785890000001</v>
+        <v>1.5209354500000001</v>
       </c>
       <c r="B5">
-        <v>2.4539716789999999</v>
+        <v>0.94678173200000004</v>
+      </c>
+      <c r="D5">
+        <v>1.571012791</v>
+      </c>
+      <c r="E5">
+        <v>6.2674740000000003E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.5856842099999999</v>
+      </c>
+      <c r="B6">
+        <v>0.86914396000000005</v>
+      </c>
+      <c r="D6">
+        <v>1.5981794899999999</v>
+      </c>
+      <c r="E6">
+        <v>-0.71560431400000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.5990193020000001</v>
+      </c>
+      <c r="B7">
+        <v>-0.25382832700000002</v>
+      </c>
+      <c r="D7">
+        <v>1.716910758</v>
+      </c>
+      <c r="E7">
+        <v>0.110969495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.666065028</v>
+      </c>
+      <c r="B8">
+        <v>1.0501666460000001</v>
+      </c>
+      <c r="D8">
+        <v>1.7991717709999999</v>
+      </c>
+      <c r="E8">
+        <v>0.473503489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.7490675929999999</v>
+      </c>
+      <c r="B9">
+        <v>0.48787993299999999</v>
+      </c>
+      <c r="D9">
+        <v>1.8093830630000001</v>
+      </c>
+      <c r="E9">
+        <v>-1.09224725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1.844634624</v>
+      </c>
+      <c r="B10">
+        <v>-0.36900263599999999</v>
+      </c>
+      <c r="D10">
+        <v>1.8783875750000001</v>
+      </c>
+      <c r="E10">
+        <v>-0.99794760900000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2.2295364069999999</v>
+      </c>
+      <c r="B11">
+        <v>2.4105133000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3.448862278</v>
+      </c>
+      <c r="B12">
+        <v>-1.329382168</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D3:E4">
-    <sortCondition ref="D3:D4"/>
+  <sortState ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>